<commit_message>
update rhombus position calculator
</commit_message>
<xml_diff>
--- a/rhombus_position_calculator.xlsx
+++ b/rhombus_position_calculator.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="24">
   <si>
     <t>Калькулятор положений ромбов на главной странице сайта</t>
   </si>
@@ -65,6 +65,27 @@
   </si>
   <si>
     <t>width, height квадрата для образования большого ромба</t>
+  </si>
+  <si>
+    <t>Положение большого ромба</t>
+  </si>
+  <si>
+    <t>small top</t>
+  </si>
+  <si>
+    <t>small left</t>
+  </si>
+  <si>
+    <t>big top</t>
+  </si>
+  <si>
+    <t>big left</t>
+  </si>
+  <si>
+    <t>положение обычного ромба, на место которого становится большой ромб</t>
+  </si>
+  <si>
+    <t>высота большого ромба (диагональ) - такой высоты делать картинки для размещения в ромбе</t>
   </si>
 </sst>
 </file>
@@ -165,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,6 +202,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -484,11 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O31"/>
+  <dimension ref="B3:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -520,7 +546,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <f>-B13/2-B20/2</f>
+        <f>-B13/2-B21/2</f>
         <v>-148.49242404917499</v>
       </c>
       <c r="C9" t="s">
@@ -529,7 +555,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
-        <f>-B13/2+B20/2</f>
+        <f>-B13/2+B21/2</f>
         <v>-131.52186130069782</v>
       </c>
       <c r="C10" t="s">
@@ -551,441 +577,497 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="B14" s="3">
+        <f>SQRT(2*B7*2*B7*2)</f>
+        <v>560.02857069974561</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
         <f>B13-TRUNC(B13)</f>
         <v>1.4285349872807274E-2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16">
         <f>B7+B8</f>
         <v>210</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17">
         <f>B7*2+B8</f>
         <v>408</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18">
         <f>B8</f>
         <v>12</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
         <f>SQRT(2*B8*B8)</f>
         <v>16.970562748477139</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I22" s="3"/>
-    </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="8">
-        <f>B9+($B$13+$B$20)/2-($B$7+$B$17)/2</f>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="8">
+        <f>B9+($B$13+$B$21)/2-($B$7+$B$18)/2</f>
         <v>-105</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="8">
-        <f>C24</f>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="8">
+        <f>C25</f>
         <v>-105</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="8">
-        <f>E24</f>
+      <c r="F25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="8">
+        <f>E25</f>
         <v>-105</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="8">
-        <f>G24</f>
+      <c r="H25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="8">
+        <f>G25</f>
         <v>-105</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="8">
-        <f>I24</f>
+      <c r="J25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="8">
+        <f>I25</f>
         <v>-105</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" s="8">
-        <f>K24</f>
+      <c r="L25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="8">
+        <f>K25</f>
         <v>-105</v>
       </c>
-      <c r="N24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O24" s="8">
-        <f>M24</f>
+      <c r="N25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="8">
+        <f>M25</f>
         <v>-105</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="7">
-        <f>B10+($B$13+$B$20)/2-($B$7+$B$17)/2</f>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="7">
+        <f>B10+($B$13+$B$21)/2-($B$7+$B$18)/2</f>
         <v>-88.029437251522836</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="7">
+        <f>C26+$B$13</f>
+        <v>191.98484809834997</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="7">
+        <f>E26+$B$13</f>
+        <v>471.99913344822278</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="7">
+        <f>G26+$B$13</f>
+        <v>752.01341879809559</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="7">
+        <f>I26+$B$13</f>
+        <v>1032.0277041479685</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26" s="7">
+        <f>K26+$B$13</f>
+        <v>1312.0419894978413</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="7">
+        <f>M26+$B$13</f>
+        <v>1592.0562748477141</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="8">
+        <f>C25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="8">
+        <f>E25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="8">
+        <f>G25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="8">
+        <f>I25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="8">
+        <f>K25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="8">
+        <f>M25+$B$13/2</f>
+        <v>35.007142674936404</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="7">
+        <f>C26+$B$13/2</f>
+        <v>51.977705423413568</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="7">
+        <f>E26+$B$13/2</f>
+        <v>331.99199077328637</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="7">
+        <f>G26+$B$13/2</f>
+        <v>612.00627612315918</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="7">
+        <f>I26+$B$13/2</f>
+        <v>892.02056147303199</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="7">
+        <f>K26+$B$13/2</f>
+        <v>1172.0348468229049</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="7">
+        <f>M26+$B$13/2</f>
+        <v>1452.0491321727777</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="8">
         <f>C25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="8">
+        <f>E25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="8">
+        <f>G25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="8">
+        <f>I25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="8">
+        <f>K25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" s="8">
+        <f>M25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="8">
+        <f>O25+$B$13</f>
+        <v>175.01428534987281</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7">
+        <f>C26</f>
+        <v>-88.029437251522836</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="7">
+        <f>E26</f>
         <v>191.98484809834997</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="7">
-        <f>E25+$B$13</f>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="7">
+        <f>G26</f>
         <v>471.99913344822278</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="7">
-        <f>G25+$B$13</f>
+      <c r="H30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="7">
+        <f>I26</f>
         <v>752.01341879809559</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="7">
-        <f>I25+$B$13</f>
+      <c r="J30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="7">
+        <f>K26</f>
         <v>1032.0277041479685</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M25" s="7">
-        <f>K25+$B$13</f>
+      <c r="L30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="7">
+        <f>M26</f>
         <v>1312.0419894978413</v>
       </c>
-      <c r="N25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O25" s="7">
-        <f>M25+$B$13</f>
+      <c r="N30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="7">
+        <f>O26</f>
         <v>1592.0562748477141</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="8">
-        <f>C24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="8">
-        <f>E24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="8">
-        <f>G24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J26" s="8">
-        <f>I24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L26" s="8">
-        <f>K24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N26" s="8">
-        <f>M24+$B$13/2</f>
-        <v>35.007142674936404</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="7">
-        <f>C25+$B$13/2</f>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="8">
+        <f>D27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="8">
+        <f>F27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="8">
+        <f>H27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="8">
+        <f>J27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="8">
+        <f>L27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" s="8">
+        <f>N27+$B$13</f>
+        <v>315.02142802480921</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="7">
+        <f>D28</f>
         <v>51.977705423413568</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="7">
-        <f>E25+$B$13/2</f>
+      <c r="E32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="7">
+        <f>F28</f>
         <v>331.99199077328637</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="7">
-        <f>G25+$B$13/2</f>
+      <c r="G32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="7">
+        <f>H28</f>
         <v>612.00627612315918</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="7">
-        <f>I25+$B$13/2</f>
+      <c r="I32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="7">
+        <f>J28</f>
         <v>892.02056147303199</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="7">
-        <f>K25+$B$13/2</f>
+      <c r="K32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L32" s="7">
+        <f>L28</f>
         <v>1172.0348468229049</v>
       </c>
-      <c r="M27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N27" s="7">
-        <f>M25+$B$13/2</f>
+      <c r="M32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" s="7">
+        <f>N28</f>
         <v>1452.0491321727777</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="8">
-        <f>C24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="8">
-        <f>E24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="8">
-        <f>G24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="8">
-        <f>I24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="8">
-        <f>K24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M28" s="8">
-        <f>M24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="8">
-        <f>O24+$B$13</f>
-        <v>175.01428534987281</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="7">
-        <f>C25</f>
-        <v>-88.029437251522836</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="7">
-        <f>E25</f>
-        <v>191.98484809834997</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="7">
-        <f>G25</f>
-        <v>471.99913344822278</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="7">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="11">
         <f>I25</f>
+        <v>-105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="11">
+        <f>I26</f>
         <v>752.01341879809559</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="7">
-        <f>K25</f>
-        <v>1032.0277041479685</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M29" s="7">
-        <f>M25</f>
-        <v>1312.0419894978413</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O29" s="7">
-        <f>O25</f>
-        <v>1592.0562748477141</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="8">
-        <f>D26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="8">
-        <f>F26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="8">
-        <f>H26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="8">
-        <f>J26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L30" s="8">
-        <f>L26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N30" s="8">
-        <f>N26+$B$13</f>
-        <v>315.02142802480921</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="7">
-        <f>D27</f>
-        <v>51.977705423413568</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="7">
-        <f>F27</f>
-        <v>331.99199077328637</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="7">
-        <f>H27</f>
-        <v>612.00627612315918</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="7">
-        <f>J27</f>
-        <v>892.02056147303199</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L31" s="7">
-        <f>L27</f>
-        <v>1172.0348468229049</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N31" s="7">
-        <f>N27</f>
-        <v>1452.0491321727777</v>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="8">
+        <f>C35+($B$13-$B$7)/2</f>
+        <v>-63.992857325063596</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="7">
+        <f>C36-$B$7/2</f>
+        <v>653.01341879809559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rhombuses styles for screen width from 992px to 1200px
</commit_message>
<xml_diff>
--- a/rhombus_position_calculator.xlsx
+++ b/rhombus_position_calculator.xlsx
@@ -136,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -188,11 +188,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,6 +313,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -521,7 +661,7 @@
   <dimension ref="B3:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +795,7 @@
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
@@ -664,39 +804,39 @@
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="20">
         <f>B9+($B$13+$B$22)/2-$B$7/2-$B$19</f>
         <v>-135</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="8">
+      <c r="D26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="17">
         <f>C26</f>
         <v>-135</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="8">
+      <c r="F26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="17">
         <f>E26</f>
         <v>-135</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="8">
+      <c r="H26" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="20">
         <f>G26</f>
         <v>-135</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="8">
+      <c r="J26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="17">
         <f>I26</f>
         <v>-135</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="12" t="s">
         <v>12</v>
       </c>
       <c r="M26" s="8">
@@ -711,43 +851,43 @@
         <v>-135</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="23">
         <f>B10+($B$13+$B$22)/2-$B$7/2-$B$19</f>
         <v>-96.514718625761418</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="19">
         <f>C27+$B$13+$B$22</f>
         <v>183.49956672411142</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="F27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="19">
         <f>E27+$B$13+$B$22</f>
         <v>463.51385207398425</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="7">
+      <c r="H27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="23">
         <f>G27+$B$13+$B$22</f>
         <v>743.52813742385717</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="7">
+      <c r="J27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="19">
         <f>I27+$B$13+$B$22</f>
         <v>1023.54242277373</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="M27" s="7">
@@ -766,18 +906,18 @@
       <c r="C28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="21">
         <f>C26+($B$13+$B$22)/2</f>
         <v>5.0071426749364321</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="E28" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="25">
         <f>E26+($B$13+$B$22)/2</f>
         <v>5.0071426749364321</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="22" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="8">
@@ -787,11 +927,11 @@
       <c r="I28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28" s="14">
         <f>I26+($B$13+$B$22)/2</f>
         <v>5.0071426749364321</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="K28" s="15" t="s">
         <v>12</v>
       </c>
       <c r="L28" s="8">
@@ -806,22 +946,22 @@
         <v>5.0071426749364321</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="21">
         <f>C27+($B$13+$B$22)/2</f>
         <v>43.492424049175014</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="7">
+      <c r="E29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="19">
         <f>E27+($B$13+$B$22)/2</f>
         <v>323.50670939904785</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="22" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="7">
@@ -831,11 +971,11 @@
       <c r="I29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="14">
         <f>I27+($B$13+$B$22)/2</f>
         <v>883.53528009879358</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="15" t="s">
         <v>13</v>
       </c>
       <c r="L29" s="7">
@@ -854,39 +994,39 @@
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="20">
         <f>C26+$B$13+$B$22</f>
         <v>145.01428534987284</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="8">
+      <c r="D30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="17">
         <f>E26+$B$13+$B$22</f>
         <v>145.01428534987284</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="8">
+      <c r="F30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="17">
         <f>G26+$B$13+$B$22</f>
         <v>145.01428534987284</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="8">
+      <c r="H30" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="20">
         <f>I26+$B$13+$B$22</f>
         <v>145.01428534987284</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="8">
+      <c r="J30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="17">
         <f>K26+$B$13+$B$22</f>
         <v>145.01428534987284</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="12" t="s">
         <v>12</v>
       </c>
       <c r="M30" s="8">
@@ -901,43 +1041,43 @@
         <v>145.01428534987284</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="21">
         <f>C27</f>
         <v>-96.514718625761418</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D31" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="19">
         <f>E27</f>
         <v>183.49956672411142</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="7">
+      <c r="F31" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="19">
         <f>G27</f>
         <v>463.51385207398425</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="7">
+      <c r="H31" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="21">
         <f>I27</f>
         <v>743.52813742385717</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" s="7">
+      <c r="J31" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="19">
         <f>K27</f>
         <v>1023.54242277373</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="22" t="s">
         <v>13</v>
       </c>
       <c r="M31" s="7">
@@ -953,42 +1093,42 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="8">
+      <c r="C32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="17">
         <f>D28+$B$13+$B$22</f>
         <v>285.02142802480932</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="8">
+      <c r="E32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="17">
         <f>F28+$B$13+$B$22</f>
         <v>285.02142802480932</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="8">
+      <c r="G32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="17">
         <f>H28+$B$13+$B$22</f>
         <v>285.02142802480932</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="8">
+      <c r="I32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="17">
         <f>J28+$B$13+$B$22</f>
         <v>285.02142802480932</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L32" s="8">
+      <c r="K32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="17">
         <f>L28+$B$13+$B$22</f>
         <v>285.02142802480932</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="M32" s="12" t="s">
         <v>12</v>
       </c>
       <c r="N32" s="8">
@@ -996,43 +1136,43 @@
         <v>285.02142802480932</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="7">
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="19">
         <f>D29</f>
         <v>43.492424049175014</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="7">
+      <c r="E33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="19">
         <f>F29</f>
         <v>323.50670939904785</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="7">
+      <c r="G33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="19">
         <f>H29</f>
         <v>603.52099474892066</v>
       </c>
-      <c r="I33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33" s="7">
+      <c r="I33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="19">
         <f>J29</f>
         <v>883.53528009879358</v>
       </c>
-      <c r="K33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="7">
+      <c r="K33" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="19">
         <f>L29</f>
         <v>1163.5495654486665</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="M33" s="13" t="s">
         <v>13</v>
       </c>
       <c r="N33" s="7">

</xml_diff>